<commit_message>
Update data.xlsx with latest results
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32032714-D1C6-42F9-9448-437E52D16CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43534426-557B-411F-818C-2BADCA8BCBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0AFDD312-DCBE-40DE-9851-59625C1673A3}"/>
   </bookViews>
@@ -22921,12 +22921,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC093899-43B0-4F81-BD69-3179AA640D8E}">
   <dimension ref="A1:Y1115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1071" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="A199" sqref="A199:XFD199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="32.21875" customWidth="1"/>
     <col min="23" max="23" width="8.88671875" style="1"/>
   </cols>
   <sheetData>

</xml_diff>